<commit_message>
Update blank v3 with new header
</commit_message>
<xml_diff>
--- a/examples/blank_v3_raw_reads.xlsx
+++ b/examples/blank_v3_raw_reads.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azyoud.EBI\Documents\EBI\COVID19_data_portal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astaffer/Repos/covid-excel-utils/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F15898F-6CFE-45B3-B477-0CC4226473F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7AF2316B-F1D6-474B-982A-A25AF0A6D3E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2355" windowWidth="29040" windowHeight="15840" xr2:uid="{23BF9E83-3E3B-E240-A0C0-6442028F11EC}"/>
+    <workbookView xWindow="28680" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{23BF9E83-3E3B-E240-A0C0-6442028F11EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="512">
   <si>
     <t>Study</t>
   </si>
@@ -120,9 +119,6 @@
     <t>collector name</t>
   </si>
   <si>
-    <t>collecting institute</t>
-  </si>
-  <si>
     <t>isolate</t>
   </si>
   <si>
@@ -205,9 +201,6 @@
   </si>
   <si>
     <t>O</t>
-  </si>
-  <si>
-    <t>#Accepted values/format</t>
   </si>
   <si>
     <t>YYYY-MM-DD</t>
@@ -1579,6 +1572,156 @@
   <si>
     <t xml:space="preserve">drag and drop uploader tool </t>
   </si>
+  <si>
+    <t>Sequencing Platform</t>
+  </si>
+  <si>
+    <t>LS454</t>
+  </si>
+  <si>
+    <t>ILLUMINA</t>
+  </si>
+  <si>
+    <t>PACBIO_SMRT</t>
+  </si>
+  <si>
+    <t>ION_TORRENT</t>
+  </si>
+  <si>
+    <t>CAPILLARY</t>
+  </si>
+  <si>
+    <t>OXFORD_NANOPORE</t>
+  </si>
+  <si>
+    <t>BGISEQ</t>
+  </si>
+  <si>
+    <t>DNBSEQ</t>
+  </si>
+  <si>
+    <t>Library Source</t>
+  </si>
+  <si>
+    <t>GENOMIC</t>
+  </si>
+  <si>
+    <t>GENOMIC SINGLE CELL</t>
+  </si>
+  <si>
+    <t>TRANSCRIPTOMIC</t>
+  </si>
+  <si>
+    <t>TRANSCRIPTOMIC SINGLE CELL</t>
+  </si>
+  <si>
+    <t>METAGENOMIC</t>
+  </si>
+  <si>
+    <t>METATRANSCRIPTOMIC</t>
+  </si>
+  <si>
+    <t>SYNTHETIC</t>
+  </si>
+  <si>
+    <t>VIRAL RNA</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>PRJEB ### or ERP ####</t>
+  </si>
+  <si>
+    <t>EMBL-EBI</t>
+  </si>
+  <si>
+    <t>COV-2</t>
+  </si>
+  <si>
+    <t>C130</t>
+  </si>
+  <si>
+    <t>ERS### or SAMEA###</t>
+  </si>
+  <si>
+    <t>severe acute respiratory syndrome coronavirus 2</t>
+  </si>
+  <si>
+    <t>Sc222</t>
+  </si>
+  <si>
+    <t>COVID19-S1</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>Healthy</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>homo sapien</t>
+  </si>
+  <si>
+    <t>John Smith</t>
+  </si>
+  <si>
+    <t>EMBL-EBI, Cambridge, UK</t>
+  </si>
+  <si>
+    <t>nasopharyngeal</t>
+  </si>
+  <si>
+    <t>55.3781° N</t>
+  </si>
+  <si>
+    <t>3.4360° W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hinxton-Cambridgeshire  </t>
+  </si>
+  <si>
+    <t>active surveillance in response to outbreak</t>
+  </si>
+  <si>
+    <t>recovered</t>
+  </si>
+  <si>
+    <t>60 IU/L</t>
+  </si>
+  <si>
+    <t>S. enterica serotype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wild </t>
+  </si>
+  <si>
+    <t>tracheal tissue</t>
+  </si>
+  <si>
+    <t>domestic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epithelial </t>
+  </si>
+  <si>
+    <t>Cov-seq103</t>
+  </si>
+  <si>
+    <t>small RNA seq</t>
+  </si>
+  <si>
+    <t>smith@ebi.ac.uk</t>
+  </si>
+  <si>
+    <t>#Accepted values/format/examples</t>
+  </si>
+  <si>
+    <t>collecting institution</t>
+  </si>
 </sst>
 </file>
 
@@ -1587,7 +1730,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1638,8 +1781,30 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1693,8 +1858,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1717,12 +1888,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1746,17 +1931,62 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="12">
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1938,30 +2168,50 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B76A0E47-097D-EB4B-9C30-8E64BCA44C8A}" name="Table1" displayName="Table1" ref="A1:A44" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B76A0E47-097D-EB4B-9C30-8E64BCA44C8A}" name="Table1" displayName="Table1" ref="A1:A44" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:A44" xr:uid="{92862242-5D97-EA45-9FF1-161A012080F3}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{23058E6F-520E-D04E-BFC8-ADD2BE9E74E2}" name="Sequencing Instrument" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{23058E6F-520E-D04E-BFC8-ADD2BE9E74E2}" name="Sequencing Instrument" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5FC20DD1-555F-5543-AE17-D7A4848BA01C}" name="Table2" displayName="Table2" ref="C1:C32" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="C1:C32" xr:uid="{E9889673-94C7-8C48-9D9D-3ED629695D0D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5FC20DD1-555F-5543-AE17-D7A4848BA01C}" name="Table2" displayName="Table2" ref="G1:G32" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="G1:G32" xr:uid="{E9889673-94C7-8C48-9D9D-3ED629695D0D}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{AFE034A3-C379-974D-82E7-7FAAE8923D92}" name="Library Selection" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{AFE034A3-C379-974D-82E7-7FAAE8923D92}" name="Library Selection" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{819ACDF6-9ECB-3D4A-A19B-67249D0F5E12}" name="Table3" displayName="Table3" ref="E1:E37" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="E1:E37" xr:uid="{816AB87E-6915-8849-B9CD-0C69266DDCB7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{819ACDF6-9ECB-3D4A-A19B-67249D0F5E12}" name="Table3" displayName="Table3" ref="I1:I37" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="I1:I37" xr:uid="{816AB87E-6915-8849-B9CD-0C69266DDCB7}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{92A8635E-BB70-364E-9CE9-F93D41FCB4AD}" name="Library Strategy" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{92A8635E-BB70-364E-9CE9-F93D41FCB4AD}" name="Library Strategy" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{14C6E254-9D74-4BC0-9EE4-4421A3F5B597}" name="Table5" displayName="Table5" ref="C1:C9" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="C1:C9" xr:uid="{5A21C853-DDB4-47F0-864C-950E47858A68}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{1040D220-6F55-4511-B1F9-0C7EF7828553}" name="Sequencing Platform"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BEEB32D0-5F50-4A44-81C1-3EE90054E470}" name="Table7" displayName="Table7" ref="E1:E10" totalsRowShown="0">
+  <autoFilter ref="E1:E10" xr:uid="{040E6671-55E0-44A8-81D5-922BB0D3FF33}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{6AF305CE-D5F3-4176-B629-65078A2965A6}" name="Library Source"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2264,64 +2514,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAF0ECBC-C68B-874D-9EA3-56F77697927C}">
-  <dimension ref="A1:BA14"/>
+  <dimension ref="A1:BA35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AY1" sqref="AY1:AY1048576"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="123.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="2"/>
-    <col min="4" max="4" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="123" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="2"/>
-    <col min="9" max="9" width="22.58203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="26.83203125" style="2" customWidth="1"/>
     <col min="10" max="10" width="12.33203125" style="20" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.83203125" style="5"/>
     <col min="14" max="14" width="14.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.75" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.58203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5" style="28" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="36.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.58203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.5" style="5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.75" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10.83203125" style="5"/>
     <col min="23" max="23" width="18.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="13.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.83203125" style="5"/>
-    <col min="26" max="26" width="22.58203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.83203125" style="5"/>
-    <col min="28" max="28" width="33.58203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="24.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="33.5" style="21" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="26.5" style="5" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="28.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="36.08203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="20.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.58203125" style="5" customWidth="1"/>
-    <col min="35" max="35" width="13.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="31.08203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="40.25" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="36" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="20.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.5" style="5" customWidth="1"/>
+    <col min="35" max="35" width="13.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="31" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="40.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="11" style="5"/>
     <col min="39" max="39" width="30" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="41" width="11" style="5"/>
+    <col min="40" max="40" width="14.83203125" style="5" customWidth="1"/>
+    <col min="41" max="41" width="11" style="5"/>
     <col min="42" max="42" width="17" style="8" bestFit="1" customWidth="1"/>
-    <col min="43" max="47" width="11" style="8"/>
+    <col min="43" max="44" width="11" style="8"/>
+    <col min="45" max="45" width="14.6640625" style="8" customWidth="1"/>
+    <col min="46" max="47" width="15.5" style="8" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="14.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11" style="8"/>
+    <col min="49" max="49" width="14.6640625" style="8" customWidth="1"/>
     <col min="50" max="50" width="52.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="22.58203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.58203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="30.25" style="8" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="22.5" style="8" customWidth="1"/>
+    <col min="52" max="52" width="13.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="30.1640625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -2342,7 +2595,7 @@
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
       <c r="P1" s="7"/>
-      <c r="Q1" s="21"/>
+      <c r="Q1" s="26"/>
       <c r="R1" s="7"/>
       <c r="S1" s="7"/>
       <c r="T1" s="7"/>
@@ -2353,7 +2606,7 @@
       <c r="Y1" s="7"/>
       <c r="Z1" s="7"/>
       <c r="AA1" s="7"/>
-      <c r="AB1" s="24" t="s">
+      <c r="AB1" s="22" t="s">
         <v>3</v>
       </c>
       <c r="AC1" s="13"/>
@@ -2384,7 +2637,7 @@
       <c r="AZ1" s="10"/>
       <c r="BA1" s="10"/>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>4</v>
@@ -2408,7 +2661,7 @@
         <v>10</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="J2" s="19" t="s">
         <v>11</v>
@@ -2431,7 +2684,7 @@
       <c r="P2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="22" t="s">
+      <c r="Q2" s="27" t="s">
         <v>18</v>
       </c>
       <c r="R2" s="6" t="s">
@@ -2456,320 +2709,400 @@
         <v>25</v>
       </c>
       <c r="Y2" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="AA2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="6" t="s">
-        <v>462</v>
-      </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AB2" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE2" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL2" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM2" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AO2" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC2" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="AD2" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE2" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF2" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG2" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH2" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI2" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ2" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK2" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="AL2" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="AM2" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="AN2" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO2" s="13" t="s">
+      <c r="AQ2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AR2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AS2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="AT2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AU2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AV2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="AW2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AX2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AY2" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="AZ2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="BA2" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AP2" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="AQ2" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="AR2" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="AS2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="AT2" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="AU2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AV2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="AW2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AX2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="AY2" s="9" t="s">
-        <v>462</v>
-      </c>
-      <c r="AZ2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="BA2" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="E3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="L3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q3" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA3" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB3" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC3" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD3" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE3" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="AF3" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="AG3" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="AH3" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="AI3" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="AJ3" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="AK3" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="AL3" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="AM3" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="AN3" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="AO3" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="AP3" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ3" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR3" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS3" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="AT3" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU3" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AV3" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AW3" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q3" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="V3" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="W3" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="X3" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y3" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="Z3" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA3" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="AB3" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="AC3" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="AD3" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="AE3" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="AF3" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="AG3" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="AH3" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="AI3" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="AJ3" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="AK3" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="AL3" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="AM3" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="AN3" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="AO3" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="AP3" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ3" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AR3" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AS3" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="AT3" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AU3" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AV3" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AW3" s="10" t="s">
-        <v>54</v>
-      </c>
       <c r="AX3" s="10" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="AY3" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AZ3" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="BA3" s="10" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.35">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+        <v>510</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>509</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>483</v>
+      </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="I4" s="4" t="s">
+        <v>461</v>
+      </c>
       <c r="J4" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
+        <v>54</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="M4" s="7">
+        <v>2697049</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>486</v>
+      </c>
       <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC4" s="14"/>
-      <c r="AD4" s="14"/>
-      <c r="AE4" s="14"/>
-      <c r="AF4" s="14"/>
-      <c r="AG4" s="14"/>
-      <c r="AH4" s="14"/>
+      <c r="P4" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="Q4" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="T4" s="7">
+        <v>131</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="Z4" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="AA4" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="AB4" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC4" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="AD4" s="14" t="s">
+        <v>497</v>
+      </c>
+      <c r="AE4" s="14" t="s">
+        <v>498</v>
+      </c>
+      <c r="AF4" s="14" t="s">
+        <v>499</v>
+      </c>
+      <c r="AG4" s="14" t="s">
+        <v>500</v>
+      </c>
+      <c r="AH4" s="14">
+        <v>46</v>
+      </c>
       <c r="AI4" s="14"/>
-      <c r="AJ4" s="14"/>
-      <c r="AK4" s="14"/>
-      <c r="AL4" s="14"/>
-      <c r="AM4" s="14"/>
-      <c r="AN4" s="14"/>
-      <c r="AO4" s="14"/>
-      <c r="AP4" s="10"/>
-      <c r="AQ4" s="10"/>
-      <c r="AR4" s="10"/>
-      <c r="AS4" s="10"/>
-      <c r="AT4" s="10"/>
-      <c r="AU4" s="10"/>
-      <c r="AV4" s="10"/>
+      <c r="AJ4" s="14" t="s">
+        <v>501</v>
+      </c>
+      <c r="AK4" s="14" t="s">
+        <v>502</v>
+      </c>
+      <c r="AL4" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="AM4" s="14" t="s">
+        <v>504</v>
+      </c>
+      <c r="AN4" s="14" t="s">
+        <v>505</v>
+      </c>
+      <c r="AO4" s="14" t="s">
+        <v>506</v>
+      </c>
+      <c r="AP4" s="10" t="s">
+        <v>507</v>
+      </c>
+      <c r="AQ4" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="AR4" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS4" s="10" t="s">
+        <v>508</v>
+      </c>
+      <c r="AT4" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="AU4" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="AV4" s="10" t="s">
+        <v>138</v>
+      </c>
       <c r="AW4" s="10"/>
       <c r="AX4" s="10"/>
       <c r="AY4" s="10"/>
       <c r="AZ4" s="10"/>
       <c r="BA4" s="10"/>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -2778,9 +3111,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="4" t="s">
-        <v>463</v>
-      </c>
+      <c r="I5" s="4"/>
       <c r="J5" s="18"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
@@ -2788,7 +3119,7 @@
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
-      <c r="Q5" s="21"/>
+      <c r="Q5" s="26"/>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
@@ -2797,21 +3128,21 @@
       <c r="W5" s="7"/>
       <c r="X5" s="7"/>
       <c r="Y5" s="7"/>
-      <c r="Z5" s="7" t="s">
-        <v>463</v>
-      </c>
+      <c r="Z5" s="7"/>
       <c r="AA5" s="7"/>
-      <c r="AB5" s="25"/>
+      <c r="AB5" s="23"/>
       <c r="AC5" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AD5" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AE5" s="14"/>
       <c r="AF5" s="14"/>
       <c r="AG5" s="14"/>
-      <c r="AH5" s="14"/>
+      <c r="AH5" s="14" t="s">
+        <v>480</v>
+      </c>
       <c r="AI5" s="14"/>
       <c r="AJ5" s="14"/>
       <c r="AK5" s="14"/>
@@ -2829,2029 +3160,2003 @@
       <c r="AW5" s="10"/>
       <c r="AX5" s="10"/>
       <c r="AY5" s="10" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="AZ5" s="10"/>
       <c r="BA5" s="10"/>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="D6" s="31"/>
+      <c r="J6" s="30"/>
+      <c r="Q6" s="29"/>
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="Q7" s="29"/>
+    </row>
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="9" spans="1:53" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+      <c r="Q8" s="29"/>
+    </row>
+    <row r="9" spans="1:53" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="10" spans="1:53" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+      <c r="Q9" s="29"/>
+    </row>
+    <row r="10" spans="1:53" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="11" spans="1:53" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+        <v>458</v>
+      </c>
+      <c r="Q10" s="29"/>
+    </row>
+    <row r="11" spans="1:53" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.35">
+        <v>459</v>
+      </c>
+      <c r="Q11" s="29"/>
+    </row>
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
+        <v>455</v>
+      </c>
+      <c r="Q12" s="29"/>
+    </row>
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
+        <v>456</v>
+      </c>
+      <c r="Q13" s="29"/>
+    </row>
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
-        <v>459</v>
-      </c>
+      <c r="Q14" s="29"/>
+    </row>
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="Q15" s="29"/>
+    </row>
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="Q16" s="29"/>
+    </row>
+    <row r="17" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q17" s="29"/>
+    </row>
+    <row r="18" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q18" s="29"/>
+    </row>
+    <row r="19" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q19" s="29"/>
+    </row>
+    <row r="20" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q20" s="29"/>
+    </row>
+    <row r="21" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q21" s="29"/>
+    </row>
+    <row r="22" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q22" s="29"/>
+    </row>
+    <row r="23" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q23" s="29"/>
+    </row>
+    <row r="24" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q24" s="29"/>
+    </row>
+    <row r="25" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q25" s="29"/>
+    </row>
+    <row r="26" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q26" s="29"/>
+    </row>
+    <row r="27" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q27" s="29"/>
+    </row>
+    <row r="28" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q28" s="29"/>
+    </row>
+    <row r="29" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q29" s="29"/>
+    </row>
+    <row r="30" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q30" s="29"/>
+    </row>
+    <row r="31" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q31" s="29"/>
+    </row>
+    <row r="32" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q32" s="29"/>
+    </row>
+    <row r="33" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q33" s="29"/>
+    </row>
+    <row r="34" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q34" s="29"/>
+    </row>
+    <row r="35" spans="17:17" x14ac:dyDescent="0.2">
+      <c r="Q35" s="29"/>
     </row>
   </sheetData>
-  <dataValidations count="97">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please use the accepted format from the list " promptTitle="Note" prompt="Disease outcome in the host" sqref="AG2:AG1048576" xr:uid="{53079B89-B826-2548-96D5-22C3BEE1D98A}">
-      <formula1>"dead,recovered,recovered with sequelae"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="if you have pre-registered a study please enter the study accession (format: PRJEB#### or ERP####)" sqref="B1:B5" xr:uid="{4BB5B13D-9F4A-4B97-9CA6-E0EFD4852ABF}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="ensure each row sample has a unique name " sqref="L1:L5" xr:uid="{772D8E95-46A5-4001-B34D-F65CAE49C449}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="if you have pre-registered a sample please enter the study accession (format: ERS#### or SAMEA####)" sqref="K2:K5" xr:uid="{88F1D973-9990-4169-9A30-42074A43B6F7}"/>
-    <dataValidation type="whole" operator="equal" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="The Taxonomy ID for SARS-Cov-2 is : 2697049" promptTitle="Note " prompt="The NCBI taxonomy ID for SARS-CoV-2 is: 2697049" sqref="M1:M5" xr:uid="{4BDF9C59-D47E-4F96-9199-293965ED1000}">
-      <formula1>2697049</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="please make sure that the date format is as following _x000a_YYYY-MM-DD_x000a_If the date is Unknown, please provide one of the following options_x000a_not collected_x000a_not provided_x000a_restricted access" sqref="Q1" xr:uid="{72C6B0FC-A567-46A7-B824-D09643444D17}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="please use the acceptable format from the list provided " promptTitle="Host Health State" prompt="Please select from the list..._x000a_If the status is Unknown, please provide one of the following options_x000a_not applicable_x000a_not collected_x000a_not provided_x000a_restricted access" sqref="U6:U1048576" xr:uid="{E71E7F2C-D910-403B-9A53-077B4A9082F1}">
-      <formula1>"diseased,healthy,not applicable,not collected,not provided,restricted access"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please select from the list..." promptTitle="Note" prompt="Please select from the list..." sqref="V6:V1048576" xr:uid="{956C05C7-78CD-4508-AABF-D4063A6A72FD}">
-      <formula1>"female,hermaphrodite,male,neuter,other,restricted access,not applicable,not collected,not provided"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="a unique identifier by which each subject can be referred to, de-identified, e.g. #131" sqref="T1:T5" xr:uid="{6B2FD9FB-5634-404C-A082-1F1EC574992D}"/>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <dataValidations xWindow="728" yWindow="330" count="48">
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="if you have pre-registered a study please enter the study accession (format: PRJEB#### or ERP####)" sqref="B1:B1048576" xr:uid="{4BB5B13D-9F4A-4B97-9CA6-E0EFD4852ABF}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="common name of the host, e.g. human" sqref="S1:S5" xr:uid="{3114CF0F-D7AB-4FA6-A309-ED16DE2CEC5C}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="Scientific name of the natural (as opposed to laboratory) host to the organism from which sample was obtained" sqref="W1:W5" xr:uid="{70E4CAF5-4A98-491A-A8BF-F02AEE0D9F17}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="Name of the person who collected the specimen. Example: John Smith" sqref="X1:X5" xr:uid="{5EC4BF90-52A8-4BAB-A98A-3A8ABC396FEC}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Name" prompt="Name of the institution to which the person collecting the specimen belongs. Format: Institute Name, Institute Address" sqref="Y1:Y5" xr:uid="{EF46E2CB-6290-465B-BB21-5AB09CFCB1FD}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="individual isolate from which the sample was obtained" sqref="AA1:AA5" xr:uid="{12276C9A-A683-4694-AB2A-417BF328CBED}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="please add a brief discription of your sample" sqref="P1:P5" xr:uid="{E48633A2-88E4-4A1F-8404-C104DC251D60}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="Please add a unique title for your sample" sqref="O1:O5" xr:uid="{22298660-A2F0-4D2C-98F5-4BB1F99082A0}"/>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="Please include the date you would like to make your study (and all associated data) public. If you would like the study to be made public immediately, please enter the current date." sqref="J1:J5" xr:uid="{1146B8FB-3980-4E66-B122-C07A8C79FE3B}">
-      <formula1>"&gt;=COUNTIF($I$1:$I1,"""")=0"</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning " error="Please make sure there are no empty fields in this column before continuing" promptTitle="Note" prompt="Please include the date you would like to make your study (and all associated data) public. If you would like the study to be made public immediately, please enter the current date." sqref="J6:J1048576" xr:uid="{729104A9-D7F8-48C8-A519-0FA20901B40A}">
-      <formula1>COUNTIF($J$6:$J6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing" promptTitle="Note" prompt="Ensure each study has a unique name" sqref="C6:C1048576" xr:uid="{1580813F-01B4-4614-973F-22C47DB934CF}">
-      <formula1>COUNTIF($C$6:$C6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing " sqref="D6:D1048576" xr:uid="{8DAECC65-9FEF-4CC1-89D6-D2ECA0020B8C}">
-      <formula1>COUNTIF($D$6:$D6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing " promptTitle="Note" prompt="e.g. Submitting Institution" sqref="E6:E1048576" xr:uid="{B81551A3-1673-45E4-BC91-6024DDB2E907}">
-      <formula1>COUNTIF($E$6:$E6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing" promptTitle="Note" prompt="Please add a unique name for your study" sqref="F6:F1048576" xr:uid="{B765A9A4-1B5D-4247-818A-7426F8385099}">
-      <formula1>COUNTIF($F$6:$F6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing" sqref="G6:G1048576" xr:uid="{F5A99751-1DE2-4F19-83A7-5F1FEECB441F}">
-      <formula1>COUNTIF($G$6:$G6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing" promptTitle="Note" prompt="Briefly describe the goals, purpose, and scope of the Study" sqref="H6:H1048576" xr:uid="{32D6982F-C711-4B3E-AAA2-070E57374172}">
-      <formula1>COUNTIF($H$6:$H6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="ensure each row sample has a unique name" sqref="L6:L1048576" xr:uid="{C5FD2096-C9C7-4CC2-8B35-FB865D0E014F}">
-      <formula1>COUNTIF($L$6:$L6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="The Taxonomy ID for SARS-Cov-2 is : 2697049" promptTitle="Note " prompt="The NCBI taxonomy ID for SARS-CoV-2 is: 2697049" sqref="M6:M1048576" xr:uid="{C1AF1ECE-807C-4E5F-B6F6-4DCE2B4ECDA3}">
-      <formula1>2697049</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="Please add a unique title for your sample" sqref="O6:O1048576" xr:uid="{E74DAFE5-4B24-4C4A-B294-2304E1531172}">
-      <formula1>COUNTIF($O$6:$O6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="please add a brief discription of your sample" sqref="P6:P1048576" xr:uid="{17E3FD76-461C-4BEC-BF71-02AA7ED76906}">
-      <formula1>COUNTIF($P$6:$P6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="If the date is unknown, please provide one of the following options_x000a_not applicable_x000a_not collected_x000a_not provided_x000a_restricted access" sqref="Q6:Q1048576" xr:uid="{DDBFF47F-B472-45E0-821F-C1222B9B2564}">
-      <formula1>COUNTIF($Q$6:$Q6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="common name of the host, e.g. human" sqref="S6:S1048576" xr:uid="{1BAF8C0E-08EC-4BB9-B0F0-BCF31846E6E0}">
-      <formula1>COUNTIF($S$6:$S6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="a unique identifier by which each subject can be referred to, de-identified, e.g. #131" sqref="T6:T1048576" xr:uid="{D44E403B-7F0F-46F3-B543-0BC6FFCA98A6}">
-      <formula1>COUNTIF($T$6:$T6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="Scientific name of the natural (as opposed to laboratory) host to the organism from which sample was obtained" sqref="W6:W1048576" xr:uid="{7429FBE5-E6C8-46D5-B9DE-2263D8B815AD}">
-      <formula1>COUNTIF($W$6:$W6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="Name of the person who collected the specimen. Example: John Smith" sqref="X6:X1048576" xr:uid="{D94FBB2E-BAA1-42B3-84DE-B5EB883F5A48}">
-      <formula1>COUNTIF($X$6:$X6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Name" prompt="Name of the institution to which the person collecting the specimen belongs. Format: Institute Name, Institute Address" sqref="Y6:Y1048576" xr:uid="{8657AC55-74AC-45C6-A621-9445B9FAD7AA}">
-      <formula1>COUNTIF($Y$6:$Y6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="individual isolate from which the sample was obtained_x000a_If the isolate is unknown please provide one of the following _x000a_not provided _x000a_not applicable _x000a_not collected " sqref="AA6:AA1048576" xr:uid="{77353253-9CCC-412D-B696-6B61C2F6AD5C}">
-      <formula1>COUNTIF($AA$6:$AA6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="Date on which the sample was received_x000a_please use the follwing format: _x000a_YYYY-MM-DD_x000a_" sqref="AB6:AB1048576" xr:uid="{A3CA97C2-56CF-458A-9C7F-B2B62B6CC10B}">
-      <formula1>COUNTIF($AB$6:$AB6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="The geographical origin of the sample as defined by latitude and longitude. The values should be reported in decimal degrees and in WGS84 system" sqref="AC1:AD5" xr:uid="{A5FB3AB1-05F0-4D99-92FE-5E9C71D7C9B6}"/>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="The geographical origin of the sample as defined by latitude and longitude. The values should be reported in decimal degrees and in WGS84 system" sqref="AC6:AC1048576" xr:uid="{65A66E95-51E6-40AA-9268-3546AA87C726}">
-      <formula1>COUNTIF($AC$6:$AC6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing" promptTitle="Note" prompt="The geographical origin of the sample as defined by latitude and longitude. The values should be reported in decimal degrees and in WGS84 system" sqref="AD6:AD1048576" xr:uid="{1123D344-EB37-407F-B0A5-128A74BB28F4}">
-      <formula1>COUNTIF($AD$6:$AD6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="The geographical origin of the sample as defined by the specific region name followed by the locality name." sqref="AE1:AE5" xr:uid="{84E05C59-CBC5-45FA-A594-F8F44766744D}"/>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="The geographical origin of the sample as defined by the specific region name followed by the locality name." sqref="AE6:AE1048576" xr:uid="{8EF8B28E-0174-41DA-8AA0-BCAA611DDA19}">
-      <formula1>COUNTIF($AE$6:$AE6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning " error="Please use the correct format. _x000a_the accepted format is : active surveillance in response to outbreak" promptTitle="Note" prompt="Reason for the sample collection" sqref="AF6:AF1048576" xr:uid="{EA2F3C27-C5F3-48D0-9D66-C9FF43ED1B13}">
-      <formula1>"active surveillance in response to outbreak"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="age of host at the time of sampling; relevant scale depends on species and study, e.g. could be seconds for amoebae or centuries for trees" sqref="AH1:AH4" xr:uid="{15EDC91D-75E3-49BE-92A9-5C131341D6FB}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="age of host at the time of sampling; relevant scale depends on species and study, e.g. could be seconds for amoebae or centuries for trees" sqref="AH5" xr:uid="{DC9D29D8-00CB-48FF-B1D8-EF1A34D6465A}">
-      <formula1>"centuries,days,decades,hours,minutes,month,seconds,weeks,years"</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please choose a unit from the list above  " promptTitle="Note" prompt="age of host at the time of sampling; relevant scale depends on species and study, e.g. could be seconds for amoebae or centuries for trees" sqref="AH6" xr:uid="{64E9F9F4-D1AB-48DF-AAAA-B8CC3D822A7B}">
-      <formula1>COUNTIF($AH$5:$AH5,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please complete the cell above before moving to the next one_x000a_If the age is unknown please write one of the folloiwng _x000a_not provided _x000a_not applicable _x000a_not collected" promptTitle="Note" prompt="age of host at the time of sampling; relevant scale depends on species and study, e.g. could be seconds for amoebae or centuries for trees" sqref="AH7:AH1048576" xr:uid="{67297F43-7F89-4596-B508-C0AEE9E51A67}">
-      <formula1>COUNTIF($AH$6:$AH6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="Unique laboratory identifier assigned to the virus by the investigator. Strain name is not sufficient since it might not be unique due to various passsages of the same virus. Format: up to 50 alphanumeric characters" sqref="AI1:AI5" xr:uid="{F38A8E96-5328-4F50-9A59-8DC51F942937}"/>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="Unique laboratory identifier assigned to the virus by the investigator. Strain name is not sufficient since it might not be unique due to various passsages of the same virus. Format: up to 50 alphanumeric characters" sqref="AI6:AI1048576" xr:uid="{76A2E130-9B98-4D47-926B-197A9BD59AE5}">
-      <formula1>COUNTIF($AI$6:$AI6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="The cut off value used by an investigatior in determining that a sample was seropositive." sqref="AJ1:AJ5" xr:uid="{948BCBA7-FFF9-43A2-AF34-5958D4A1C3AD}"/>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="The cut off value used by an investigatior in determining that a sample was seropositive." sqref="AJ6:AJ1048576" xr:uid="{F41B6819-10A7-4F63-BC89-32B8D9FDE76B}">
-      <formula1>COUNTIF($AJ$6:$AJ6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="Serological variety of a species characterised by its antigenic properties" sqref="AK1:AK5" xr:uid="{215832FE-A2AD-4134-8A59-EE81A029C12B}"/>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="Serological variety of a species characterised by its antigenic properties" sqref="AK6:AK1048576" xr:uid="{084FF804-2C33-4F55-B7D1-8AB7E0D4B845}">
-      <formula1>COUNTIF($AK$6:$AK6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please use the accepted format from the list..." promptTitle="Note " prompt="Natural habitat of the host." sqref="AL6:AL1048576" xr:uid="{57668189-BBAF-46BF-B5D7-7B8E77F44D5F}">
-      <formula1>"domestic:free-range farm,domestic:indoor farm,domestic:live market,domestic:semi-enclosed housing,other,wild:migratory,wild:resident"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="Name of host tissue or organ sampled for analysis. Example: tracheal tissue" sqref="AM1:AM5" xr:uid="{CE059637-0D99-49D8-8E5D-EFF919D4EE40}"/>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing" promptTitle="Note" prompt="Name of host tissue or organ sampled for analysis. Example: tracheal tissue" sqref="AM6:AM1048576" xr:uid="{FA381901-49FF-4297-9357-D1AEF1D53E40}">
-      <formula1>COUNTIF($AM$6:$AM6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please use the accepted format from the list" sqref="AN6:AN1048576" xr:uid="{54BC7784-B11C-4959-B73D-6AA54FF1921C}">
-      <formula1>"captive-wild (e.g. at zoo),domestic,other,wild"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="Name of host tissue or organ sampled for the analysis " sqref="AO1:AO5" xr:uid="{170F2E4C-1C3C-49A4-A378-06D87540E7BE}"/>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="Name of host tissue or organ sampled for the analysis " sqref="AO6:AO1048576" xr:uid="{34443CCA-016E-47D5-A400-DFDA134810B4}">
-      <formula1>COUNTIF($AO$6:$AO6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="Please use a unique name for each raw " sqref="AP1:AP5" xr:uid="{917B9B88-D2E5-4C38-881D-FB066E41ABED}"/>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing" promptTitle="Note" prompt="Please use a unique name for each raw " sqref="AP6:AP1048576" xr:uid="{B7FBDF0A-890D-460E-BFBE-3B6DF56A4B20}">
-      <formula1>COUNTIF($AP$6:$AP6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please use the accepted format from the list provided..." promptTitle="Note" prompt="Please select from the list..." sqref="AQ6:AQ1048576" xr:uid="{8C95FDA6-4A84-46F1-9AFF-6BB732FFEBA6}">
-      <formula1>"LS454,ILLUMINA,PACBIO_SMRT,ION_TORRENT,CAPILLARY,OXFORD_NANOPORE,BGISEQ"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please use the accepted format from the list provided..." promptTitle="Note" prompt="Please select from the list..." sqref="AR6:AR1048576" xr:uid="{C5104450-75AC-4B3A-B5B8-757B262B124B}">
-      <formula1>SequencingInstruments</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" sqref="AS6:AS1048576" xr:uid="{AC7BB54C-40E8-49DD-975C-B48D3F94A829}">
-      <formula1>COUNTIF($AS$6:$AS6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please use the accepted format from the list provided..." promptTitle="Note" prompt="specifies the type of source material that is being sequenced._x000a_Please select from the list..." sqref="AT6:AT1048576" xr:uid="{43ABCEA6-E0A8-469E-A4C5-F622547CDED3}">
-      <formula1>"GENOMIC,GENOMIC SINGLE CELL,TRANSCRIPTOMIC,TRANSCRIPTOMIC SINGLE CELL,METAGENOMIC,METATRANSCRIPTOMIC,SYNTHETIC,VIRAL RNA,OTHER"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please use the accepted format from the list provided..." promptTitle="Note" prompt="specifies which method was used to select for, against, enrich, or screen, the material being sequenced. _x000a_Please select from the list" sqref="AU6:AU1048576" xr:uid="{ED79DFFB-83EB-4B12-B4CD-4F6836073473}">
-      <formula1>LibrarySelection</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please use the accepted format from the list provided..." promptTitle="Note" prompt="The sequencing technique intended for this library. _x000a_Please select from the list" sqref="AV6:AV1048576" xr:uid="{09F6D8E4-C9A4-4FD6-B1DF-EBE0A983D7C5}">
-      <formula1>LibraryStrategy</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note " prompt="Please include a brief discription for the library used " sqref="AW1:AW5" xr:uid="{E4B8378D-0EC0-4A83-8EAC-404B1778FB4A}"/>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note " prompt="Please include a brief discription for the library used " sqref="AW6:AW1048576" xr:uid="{EA1D9E63-28BC-4021-A557-F06453D69621}">
-      <formula1>COUNTIF($AW$6:$AW6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="Mandatory for the paired fastq and optional for single fastq" sqref="AX1" xr:uid="{2BDEB959-6D70-4291-9FA1-C37A2D181C14}"/>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="Mandatory for the paired fastq and optional for single fastq and other read data" sqref="AX6:AX1048576" xr:uid="{AAC626D5-151D-4CB6-8576-8E68365D6AF9}">
-      <formula1>COUNTIF($AX$6:$AX6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="Please add here the full file name according to the following: _x000a_in case of paired fastq : Put the name of one of the files that you have _x000a_in case of single fastq and othe raw read data : Put the name of the file that you have  _x000a_" sqref="AZ1:AZ5" xr:uid="{D8664703-3726-4CC3-A46F-AA871B11B573}"/>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="Please add here the full file name according to the following: _x000a_in case of paired fastq : Put the name of one of the files that you have _x000a_in case of single fastq and othe raw read data : Put the name of the file that you have" sqref="AZ6:AZ1048576" xr:uid="{9C5CEB8B-3AAC-4876-B99A-C5DB4C2C846C}">
-      <formula1>COUNTIF($AZ$6:$AZ6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="Please add here the full name of the second file of paired fastq._x000a_in case of single fastq and other raw read data, add : not applicable" sqref="BA1:BA5" xr:uid="{6374E7D4-C49B-4557-94E7-C3B864BDAF21}"/>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="Please add here the full name of the second file of paired fastq._x000a_in case of single fastq and other raw read data, add : not applicable" sqref="BA6:BA1048576" xr:uid="{53686BB0-C6FF-48FC-B322-5D06F2845DF8}">
-      <formula1>COUNTIF($BA$6:$BA6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="if you have pre-registered a sample please enter the study accession (format: ERS#### or SAMEA####)" sqref="K6:K1048576" xr:uid="{A0F82282-FFE4-4F17-91C5-5A15DA6CE44E}">
-      <formula1>COUNTIF($K$6:$K6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="if you have pre-registered a study please enter the study accession (format: PRJEB#### or ERP####)" sqref="B6:B1048576" xr:uid="{B2B7CC19-711B-4CC0-B57E-11AAEB68EA6F}">
-      <formula1>COUNTIF($B$6:$B6,"")=0</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please use the accepted format _x000a_Accepted format : SARS-CoV-2" promptTitle="Note" prompt="please use the accepted format: Severe acute respiratory syndrome coronavirus 2" sqref="N2:N5" xr:uid="{91C63C49-BC49-48A9-A43F-D4C17ADC5AD3}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="Ensure each study has a unique name" sqref="C1:C5" xr:uid="{726CD6F8-C17E-459B-AC01-8B6FC7DC6FF4}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="Briefly describe the goals, purpose, and scope of the Study" sqref="H1:H5 I1 Z1 AY1" xr:uid="{64949A5C-D1FC-4D2B-9493-9E37F7C059BA}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note " prompt="e.g. Submitting Institution" sqref="E1:E5" xr:uid="{4D541A4E-0AEC-4DC7-B13E-7023DE282B09}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="If the date is unknown, please provide one of the following options_x000a_not applicable_x000a_not collected_x000a_not provided_x000a_restricted access" sqref="Q2:Q5" xr:uid="{0A37EC27-C819-4AF8-91E2-933BA766839D}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="Date on which the sample was received_x000a_please use the follwing format: _x000a_YYYY-MM-DD" sqref="AB2:AB5" xr:uid="{01AB436D-34C1-4ADF-8E6E-5F6F6690E6F8}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please use the accepted format from the list..." promptTitle="Note " prompt="Natural habitat of the host." sqref="AL2:AL5" xr:uid="{691B6464-EEEA-49BF-A623-2A529A5DC642}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please use the accepted format from the list provided..." promptTitle="Note" prompt="specifies the type of source material that is being sequenced._x000a_Please select from the list..._x000a_" sqref="AT2:AT5" xr:uid="{67254258-D05B-4603-905C-EFF2694EDCA9}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please use the accepted format from the list provided..." promptTitle="Note" prompt="specifies which method was used to select for, against, enrich, or screen, the material being sequenced. _x000a_Please select from the list_x000a_" sqref="AU2:AU5" xr:uid="{6E88930C-5F8B-468D-A8F2-C36BA53FA932}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please use the accepted format from the list provided..." promptTitle="Note" prompt="The sequencing technique intended for this library. _x000a_Please select from the list" sqref="AV2:AV5" xr:uid="{B048137D-7CF5-4B6A-805C-B2E808149FAB}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="Mandatory for the paired fastq and optional for single fastq and other read data" sqref="AX2:AX5" xr:uid="{F835C478-8E54-4AFC-8A28-BF01EFB22A44}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please use the accepted format from the list provided..." promptTitle="Note" prompt="Please select from the list..." sqref="AQ2:AR5" xr:uid="{5847A90F-CA31-41A0-8FEA-2B4CE0CB15C4}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please use the accepted format from the list" sqref="AN2:AN5" xr:uid="{956EC801-CEB2-4DBE-9F4F-CCA861703138}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning " error="Please use the correct format. _x000a_the accepted format is : active surveillance in response to outbreak" promptTitle="Note" prompt="Reason for the sample collection" sqref="AF2:AF5" xr:uid="{4F08E94C-CA71-4EBD-A071-53BF056E5229}"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please select from the list..." promptTitle="Note" prompt="Please select from the list..." sqref="V2:V5" xr:uid="{1BD25A80-15FC-4F65-A895-665196F62CAA}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="please use the acceptable format from the list provided " promptTitle="Host Health State" prompt="Please select from the list..._x000a_If the status is Unknown, please provide one of the following options_x000a_not applicable_x000a_not collected_x000a_not provided_x000a_restricted access" sqref="U2:U5" xr:uid="{8F5EB750-9D8C-480F-8D5A-16A159055022}"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please include a country name from the list provided. " promptTitle="Note" prompt="Please include a country name from the list provided. _x000a_" sqref="R2:R5" xr:uid="{7EFDAE57-23AD-4805-AB9F-E51A1B5C22C3}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please use the accepted format _x000a_Accepted format : SARS-CoV-2" promptTitle="Note" prompt="please use the accepted format: Severe acute respiratory syndrome coronavirus 2" sqref="N6:N1048576" xr:uid="{7945F8AF-06D5-4C52-82C3-BFD86F159B3F}">
-      <formula1>"Severe acute respiratory syndrome coronavirus 2"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="please use the accepted value : drag and drop uploader tool " sqref="I2:I5 Z2:Z5 AY2:AY5" xr:uid="{C05B6767-BDE3-4A58-A26F-56B2C463FCF3}"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="please use the accepted value : drag and drop uploader tool " promptTitle="Note" prompt="please use the accepted value : drag and drop uploader tool " sqref="AY6:AY1048576" xr:uid="{9FD50743-3730-4307-84BA-C622A090F52F}">
-      <formula1>"drag and drop uploader tool "</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="please use the accepted value : drag and drop uploader tool " promptTitle="Note" prompt="please use the accepted value : drag and drop uploader tool " sqref="I6:I1048576 Z6:Z1048576" xr:uid="{A9B2C88A-7DA5-45E6-9C37-34EBD071771A}">
-      <formula1>"drag and drop uploader tool "</formula1>
-    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="individual isolate from which the sample was obtained" sqref="AA1:AA1048576" xr:uid="{12276C9A-A683-4694-AB2A-417BF328CBED}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please make sure there are no empty fields in this column before continuing_x000a_" promptTitle="Note" prompt="common name of the host, e.g. human" sqref="S6:S1048576" xr:uid="{1BAF8C0E-08EC-4BB9-B0F0-BCF31846E6E0}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="ensure each study has a unique name" sqref="C1:C1048576 F6" xr:uid="{9274CCFE-E5CD-4062-9DCF-B05CDB5D0350}"/>
+    <dataValidation allowBlank="1" sqref="D1:D1048576 AS1:AS1048576" xr:uid="{887EDB9B-3844-47DC-9A0B-984948E6C76A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="please add a unique name for your study" sqref="F1:F5 F7:F1048576" xr:uid="{BC510987-9A41-4FAE-8CFD-4E6AC53D5526}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="Briefly describe the goals, purpose and scope of the Study" sqref="H1:H1048576" xr:uid="{CEF83B25-65AC-4F97-B79B-238E84F33399}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="please use the accepted value: drag and drop uploader tool" sqref="Z1:Z1048576 I1:I1048576 AY1:AY1048576" xr:uid="{2F1C5FEB-8D9F-4AB9-B96E-9F11AEF68920}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="Please include the date you would like to make your study (and all associated data) public. If you would like the study to be made public immediately, please enter the current date." sqref="J1:J1048576" xr:uid="{1DDC8BB5-31A5-4643-BD40-9DFD744BD26D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="If you have pre-registered a sample please enter the study accession (e.g. ERS#### or SAMEA####)" sqref="K1:K1048576" xr:uid="{0CE1A546-A748-4104-943F-B9AFA8F5D12C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="ensure each row has a unique sample name" sqref="L1:L1048576" xr:uid="{E006F791-1FA4-4428-AE02-E87C8FAC20BB}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="The NCBI taxonomy ID for SARS-CoV-2 is: 2697049" sqref="M1:M1048576" xr:uid="{E2D16C10-6E72-4BE3-8AED-BC7A3A7C1C21}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="Please use the accepted format: Severe acute respiratory syndrome coronavirus 2" sqref="N1:N1048576" xr:uid="{A57DCDB4-A319-455C-8705-35C6171DD98C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="please add a unique title for your sample" sqref="O1:O1048576" xr:uid="{C09E58A4-6356-4771-AFA7-AE9D7AD7F599}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="please add a brief description of your sample" sqref="P1:P1048576" xr:uid="{E052A3C3-F7F3-4EC2-B130-577CB5F5228D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="please make sure that the date format is the following:_x000a_YYYY-MM-DD_x000a_If the date is unknown, please provide one of the following options:_x000a_not applicable, not collected, not provided, restricted access" sqref="Q1:Q1048576" xr:uid="{541DC319-C96D-49D4-8B7B-54648DB5C6FE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="please include a country name only" sqref="R1:R1048576" xr:uid="{E9447CB0-C98D-45D5-9AF1-D6574E48BEB8}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="A unique identifier by which each subject can be referred to, de-identified, e.g. #131" sqref="T1:T1048576" xr:uid="{ECADFB31-5481-4D0C-84BC-892815DD0546}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="If the status is unknown, please provide one of the following:_x000a_not applicable, not collected, not provided, restricted access" sqref="U1:U1048576" xr:uid="{FA8B7EB2-1ED4-46F7-8547-C9BBDDA31BB5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="please choose one of the following:_x000a_female, hermaphrodite, male, neuter, not applicable, not collected, not provided, other, restricted access" sqref="V1:V1048576" xr:uid="{C01BF32D-A8B9-4AC6-A5A9-7DFCB3A31332}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="Scientific name of the natural (as opposed to laboratory) host of the organism from which sample was obtained" sqref="W1:W1048576" xr:uid="{BCF7F833-C189-4356-8AC0-28A4D0DA8CB9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="Name of the person who collected the specimen. E.g John Smith" sqref="X1:X1048576 Y6:Y97" xr:uid="{359E3AC4-F2DB-4336-A0FD-37F509A7007D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="Name of the institution to which the person collecting the specimen belongs. Format: Institute Name, Institute Address" sqref="Y1:Y5 Y98:Y1048576" xr:uid="{20B65C1C-6895-40A4-86E0-7A5637FA885C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="please ensure each row has a unique experiment name " sqref="AP1:AP1048576" xr:uid="{29323E2B-4D99-4607-8A94-5F949606B4C8}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="Please select from the list on the 'Accepted_Values' sheet of this spreadsheet" sqref="AQ1:AQ1048576" xr:uid="{DB2D0D03-52F6-4E7A-8BC1-FDF1FBC66944}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="please select from the list on the 'Accepted_Values' sheet of this spreadsheet" sqref="AR1:AR1048576" xr:uid="{1475954F-1CEF-4CFD-B94E-4EE09AA9EF08}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="specifies the type of material being sequenced._x000a_Please select from the list on the 'Accepted_Values' sheet of this spreadsheet" sqref="AT1:AT1048576" xr:uid="{A47CE608-BD7F-47DF-8BD9-0D57E28C263C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="specifies which method was used to select for, against, enrich, or screen, the material being sequenced. _x000a_Please select from the list on the 'Accepted_Values' sheet of this spreadsheet" sqref="AU1:AU1048576" xr:uid="{8539BC2C-4011-4C23-B714-60F077500705}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="The sequencing technique intended for this library. _x000a_Please select from the list on the 'Accepted_Values' sheet of this spreadsheet" sqref="AV1:AV1048576" xr:uid="{90E43F35-EC05-42F3-8DE2-17FB5B345BF2}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="please include a brief description of the library used" sqref="AW1:AW1048576" xr:uid="{89EDE2CB-15F0-4A9F-A832-64B00D2D9AC1}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="Mandatory for the paired fastq and optional for single fastq and other read data" sqref="AX1:AX1048576" xr:uid="{0198CA1F-5DA7-4AD1-A67B-DD36B023FE81}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" prompt="Please add here the full file name according to the following: _x000a_if single fastq and other raw read data :  complete the 'uploaded file 1' column only_x000a_if paired fastq: complete both uploaded file 1 and 2 columns" sqref="AZ1:AZ1048576" xr:uid="{0D7FCD0F-7587-4286-B61F-487DBA725CE9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="Please add here the full name of the second file of paired fastq._x000a_in case of single fastq and other raw read data, add: not applicable" sqref="BA1:BA1048576" xr:uid="{06D7B121-5F41-4697-AFC1-6F34D03012E6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="date on which the sample was received. Please use the following format: YYYY-MM-DD" sqref="AB1:AB1048576" xr:uid="{1FF825A5-16A3-4517-B7E2-87619DB13D3D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="The geographical origin of the sample as defined by latitude and longitude. The values should be reported in decimal degrees and in the WGS84 system" sqref="AC1:AC1048576" xr:uid="{F64E74E9-1911-493E-9B2C-A11C6B4C0A2B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="The geographical origin of the sample as defined by latitude and longitude. The values should be reported in decimal degrees and in WGS84 system" sqref="AD1:AD1048576" xr:uid="{4EF692B0-F97A-4FFA-98B9-3539D80A7F8B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="The geographical origin of the sample as defined by the specific region name followed by the locality name" sqref="AE1:AE1048576" xr:uid="{907D95F3-823E-482D-92CD-3BE28475B982}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="Reason for sample collection. Please add active surveillance in response to outbreak" sqref="AF1:AF1048576" xr:uid="{4A1BBB62-6BE9-45EA-8075-E8B02127F192}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="Disease outcome in host. _x000a_Please choose one of the following: dead, recovered, recovered with sequelae" sqref="AG1:AG1048576" xr:uid="{0DF796D5-8D27-46A6-983D-A754D1A0256D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="age of host at the time of sampling. _x000a_Please choose from the following units: years, centuries, days, decades, hours, minutes, months, seconds, weeks_x000a_Scale depends on species and study, e.g. could be seconds for amoebae or centuries for trees" sqref="AH1:AH1048576" xr:uid="{832771EB-B22E-4B7C-A67F-7AE62FD2E6EC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note " prompt="Unique laboratory identifier assigned to the virus by the investigator. Strain name is not sufficient since it might not be unique due to various passsages of the same virus. Format: up to 50 alphanumeric characters" sqref="AI1:AI1048576" xr:uid="{F984FC1D-3E07-42D0-AFC4-12328E31532E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="The cut off value used by an investigator in determining that a sample was seropositive" sqref="AJ1:AJ1048576" xr:uid="{2421B1B7-5B9D-41B9-9412-EEE6238DB3B0}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="Serological variety of a species characterised by it's antigenic properties" sqref="AK1:AK1048576" xr:uid="{41AEAD72-DC21-46C3-8EE7-DCDFA0AC05AF}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="The natural habitat of the host._x000a_Please choose one of the following:_x000a_domestic free range farm, domestic indoor farm, domestic live market, domestic semi-enclosed housing, other, wild migratory, wild resident" sqref="AL1:AL1048576" xr:uid="{8138C133-2F79-4618-9171-C064E28BDAC3}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="Name of host organ or tissue sampled for analysis._x000a_Example: tracheal tissue" sqref="AM1:AM1048576" xr:uid="{471C72FE-7E3B-4A28-BB99-B2D586557D21}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Note" prompt="Please choose from one of the following:_x000a_captive-wild, domestic, other, wild" sqref="AN1:AN1048576" xr:uid="{04F13376-87B3-41F1-BF10-3054C6A23A67}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Note" prompt="Name of host tissue or organ sampled for the analysis" sqref="AO1:AO1048576" xr:uid="{9D82F5BD-BECE-4124-9ACC-06E04D5179AE}"/>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{C042782A-D2CD-40D0-BAFE-E5F89681A75D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Warning" error="Please include a country name from the list provided. " promptTitle="Note" prompt="Please include a country name from the list provided. _x000a_" xr:uid="{6700193D-17A2-4EE2-A2AE-1D9DEF26E152}">
-          <x14:formula1>
-            <xm:f>Accepted_Values!$H$2:$H$279</xm:f>
-          </x14:formula1>
-          <xm:sqref>R6:R1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B11CEA-3733-DD4F-85CB-DB5B67B5124E}">
-  <dimension ref="A1:H279"/>
+  <dimension ref="A1:L279"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.08203125" customWidth="1"/>
-    <col min="5" max="5" width="16.58203125" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="9" max="9" width="16.5" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>462</v>
+      </c>
+      <c r="E1" t="s">
+        <v>471</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>463</v>
+      </c>
+      <c r="E2" t="s">
+        <v>472</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="L2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C3" t="s">
+        <v>464</v>
+      </c>
+      <c r="E3" t="s">
+        <v>473</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="I3" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="L3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C4" t="s">
+        <v>465</v>
+      </c>
+      <c r="E4" t="s">
+        <v>474</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="I4" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L4" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C5" t="s">
+        <v>466</v>
+      </c>
+      <c r="E5" t="s">
+        <v>475</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="I5" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="H3" t="s">
+      <c r="L5" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C6" t="s">
+        <v>467</v>
+      </c>
+      <c r="E6" t="s">
+        <v>476</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="H4" t="s">
+      <c r="L6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C7" t="s">
+        <v>468</v>
+      </c>
+      <c r="E7" t="s">
+        <v>477</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="I7" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="H5" t="s">
+      <c r="L7" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C8" t="s">
+        <v>469</v>
+      </c>
+      <c r="E8" t="s">
+        <v>478</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="H6" t="s">
+      <c r="L8" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C9" t="s">
+        <v>470</v>
+      </c>
+      <c r="E9" t="s">
+        <v>479</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="I9" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="H7" t="s">
+      <c r="L9" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="E10" t="s">
+        <v>167</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="I10" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="H8" t="s">
+      <c r="L10" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="G11" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="I11" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="H9" t="s">
+      <c r="L11" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="G12" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="I12" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="H10" t="s">
+      <c r="L12" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="G13" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="I13" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="H11" t="s">
+      <c r="L13" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="G14" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="I14" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="H12" t="s">
+      <c r="L14" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="G15" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="I15" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="H13" t="s">
+      <c r="L15" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="G16" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="I16" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="H14" t="s">
+      <c r="L16" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="G17" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="I17" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="H15" t="s">
+      <c r="L17" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="G18" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="I18" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H16" t="s">
+      <c r="L18" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="G19" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="I19" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="H17" t="s">
+      <c r="L19" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="G20" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="I20" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="L20" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="I21" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="H18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="E19" s="11" t="s">
+      <c r="L21" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="I22" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="H19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="L22" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="G23" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="I23" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="H21" t="s">
+      <c r="L23" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="G24" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="I24" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="H22" t="s">
+      <c r="L24" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="11" t="s">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="G25" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="I25" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="H23" t="s">
+      <c r="L25" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="11" t="s">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="G26" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="I26" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="H24" t="s">
+      <c r="L26" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="11" t="s">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="G27" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="I27" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="H25" t="s">
+      <c r="L27" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="11" t="s">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="G28" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="I28" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="H26" t="s">
+      <c r="L28" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="11" t="s">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="G29" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="I29" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="H27" t="s">
+      <c r="L29" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="11" t="s">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="G30" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="I30" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="H28" t="s">
+      <c r="L30" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="11" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="G31" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="I31" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="H29" t="s">
+      <c r="L31" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="11" t="s">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E30" s="11" t="s">
+      <c r="G32" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="I32" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="H30" t="s">
+      <c r="L32" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="11" t="s">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="E31" s="11" t="s">
+      <c r="I33" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="H31" t="s">
+      <c r="L33" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="11" t="s">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C32" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="E32" s="11" t="s">
+      <c r="I34" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="H32" t="s">
+      <c r="L34" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="11" t="s">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="I35" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="H33" t="s">
+      <c r="L35" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="11" t="s">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="I36" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="H34" t="s">
+      <c r="L36" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="11" t="s">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="I37" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="H35" t="s">
+      <c r="L37" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="11" t="s">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="E36" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="H36" t="s">
+      <c r="L38" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="11" t="s">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="E37" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="H37" t="s">
+      <c r="L39" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="11" t="s">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="H38" t="s">
+      <c r="L40" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="11" t="s">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="H39" t="s">
+      <c r="L41" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" s="11" t="s">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="H40" t="s">
+      <c r="L42" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" s="11" t="s">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="H41" t="s">
+      <c r="L43" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="11" t="s">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="H42" t="s">
+      <c r="L44" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="H43" t="s">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L45" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="H44" t="s">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L46" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H45" t="s">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L47" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H46" t="s">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L48" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H47" t="s">
+    <row r="49" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L49" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H48" t="s">
+    <row r="50" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L50" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H49" t="s">
+    <row r="51" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L51" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H50" t="s">
+    <row r="52" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L52" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="51" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H51" t="s">
+    <row r="53" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L53" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="52" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H52" t="s">
+    <row r="54" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L54" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="53" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H53" t="s">
+    <row r="55" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L55" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="54" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H54" t="s">
+    <row r="56" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L56" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="55" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H55" t="s">
+    <row r="57" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L57" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="56" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H56" t="s">
+    <row r="58" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L58" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="57" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H57" t="s">
+    <row r="59" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L59" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="58" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H58" t="s">
+    <row r="60" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L60" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="59" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H59" t="s">
+    <row r="61" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L61" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="60" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H60" t="s">
+    <row r="62" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L62" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="61" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H61" t="s">
+    <row r="63" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L63" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="62" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H62" t="s">
+    <row r="64" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L64" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="63" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H63" t="s">
+    <row r="65" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L65" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="64" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H64" t="s">
+    <row r="66" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L66" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="65" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H65" t="s">
+    <row r="67" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L67" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="66" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H66" t="s">
+    <row r="68" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L68" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="67" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H67" t="s">
+    <row r="69" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L69" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="68" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H68" t="s">
+    <row r="70" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L70" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="69" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H69" t="s">
+    <row r="71" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L71" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="70" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H70" t="s">
+    <row r="72" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L72" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="71" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H71" t="s">
+    <row r="73" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L73" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="72" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H72" t="s">
+    <row r="74" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L74" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="73" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H73" t="s">
+    <row r="75" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L75" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="74" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H74" t="s">
+    <row r="76" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L76" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="75" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H75" t="s">
+    <row r="77" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L77" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="76" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H76" t="s">
+    <row r="78" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L78" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="77" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H77" t="s">
+    <row r="79" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L79" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="78" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H78" t="s">
+    <row r="80" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L80" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="79" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H79" t="s">
+    <row r="81" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L81" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="80" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H80" t="s">
+    <row r="82" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L82" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="81" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H81" t="s">
+    <row r="83" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L83" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="82" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H82" t="s">
+    <row r="84" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L84" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="83" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H83" t="s">
+    <row r="85" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L85" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="84" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H84" t="s">
+    <row r="86" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L86" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="85" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H85" t="s">
+    <row r="87" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L87" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="86" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H86" t="s">
+    <row r="88" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L88" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="87" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H87" t="s">
+    <row r="89" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L89" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="88" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H88" t="s">
+    <row r="90" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L90" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="89" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H89" t="s">
+    <row r="91" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L91" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="90" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H90" t="s">
+    <row r="92" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L92" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="91" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H91" t="s">
+    <row r="93" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L93" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="92" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H92" t="s">
+    <row r="94" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L94" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="93" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H93" t="s">
+    <row r="95" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L95" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="94" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H94" t="s">
+    <row r="96" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L96" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="95" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H95" t="s">
+    <row r="97" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L97" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="96" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H96" t="s">
+    <row r="98" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L98" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="97" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H97" t="s">
+    <row r="99" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L99" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="98" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H98" t="s">
+    <row r="100" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L100" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="99" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H99" t="s">
+    <row r="101" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L101" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="100" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H100" t="s">
+    <row r="102" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L102" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="101" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H101" t="s">
+    <row r="103" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L103" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="102" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H102" t="s">
+    <row r="104" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L104" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="103" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H103" t="s">
+    <row r="105" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L105" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="104" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H104" t="s">
+    <row r="106" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L106" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="105" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H105" t="s">
+    <row r="107" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L107" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="106" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H106" t="s">
+    <row r="108" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L108" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="107" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H107" t="s">
+    <row r="109" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L109" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="108" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H108" t="s">
+    <row r="110" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L110" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="109" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H109" t="s">
+    <row r="111" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L111" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="110" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H110" t="s">
+    <row r="112" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L112" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="111" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H111" t="s">
+    <row r="113" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L113" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="112" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H112" t="s">
+    <row r="114" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L114" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="113" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H113" t="s">
+    <row r="115" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L115" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="114" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H114" t="s">
+    <row r="116" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L116" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="115" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H115" t="s">
+    <row r="117" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L117" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="116" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H116" t="s">
+    <row r="118" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L118" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="117" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H117" t="s">
+    <row r="119" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L119" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="118" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H118" t="s">
+    <row r="120" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L120" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="119" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H119" t="s">
+    <row r="121" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L121" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="120" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H120" t="s">
+    <row r="122" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L122" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="121" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H121" t="s">
+    <row r="123" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L123" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="122" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H122" t="s">
+    <row r="124" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L124" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="123" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H123" t="s">
+    <row r="125" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L125" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="124" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H124" t="s">
+    <row r="126" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L126" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="125" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H125" t="s">
+    <row r="127" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L127" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="126" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H126" t="s">
+    <row r="128" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L128" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="127" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H127" t="s">
+    <row r="129" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L129" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="128" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H128" t="s">
+    <row r="130" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L130" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="129" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H129" t="s">
+    <row r="131" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L131" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="130" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H130" t="s">
+    <row r="132" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L132" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="131" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H131" t="s">
+    <row r="133" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L133" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="132" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H132" t="s">
+    <row r="134" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L134" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="133" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H133" t="s">
+    <row r="135" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L135" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="134" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H134" t="s">
+    <row r="136" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L136" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="135" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H135" t="s">
+    <row r="137" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L137" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="136" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H136" t="s">
+    <row r="138" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L138" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="137" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H137" t="s">
+    <row r="139" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L139" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="138" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H138" t="s">
+    <row r="140" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L140" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="139" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H139" t="s">
+    <row r="141" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L141" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="140" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H140" t="s">
+    <row r="142" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L142" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="141" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H141" t="s">
+    <row r="143" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L143" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="142" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H142" t="s">
+    <row r="144" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L144" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="143" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H143" t="s">
+    <row r="145" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L145" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="144" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H144" t="s">
+    <row r="146" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L146" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="145" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H145" t="s">
+    <row r="147" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L147" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="146" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H146" t="s">
+    <row r="148" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L148" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="147" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H147" t="s">
+    <row r="149" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L149" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="148" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H148" t="s">
+    <row r="150" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L150" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="149" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H149" t="s">
+    <row r="151" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L151" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="150" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H150" t="s">
+    <row r="152" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L152" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="151" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H151" t="s">
+    <row r="153" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L153" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="152" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H152" t="s">
+    <row r="154" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L154" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="153" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H153" t="s">
+    <row r="155" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L155" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="154" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H154" t="s">
+    <row r="156" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L156" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="155" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H155" t="s">
+    <row r="157" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L157" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="156" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H156" t="s">
+    <row r="158" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L158" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="157" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H157" t="s">
+    <row r="159" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L159" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="158" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H158" t="s">
+    <row r="160" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L160" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="159" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H159" t="s">
+    <row r="161" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L161" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="160" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H160" t="s">
+    <row r="162" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L162" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="161" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H161" t="s">
+    <row r="163" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L163" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="162" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H162" t="s">
+    <row r="164" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L164" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="163" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H163" t="s">
+    <row r="165" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L165" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="164" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H164" t="s">
+    <row r="166" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L166" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="165" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H165" t="s">
+    <row r="167" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L167" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="166" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H166" t="s">
+    <row r="168" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L168" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="167" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H167" t="s">
+    <row r="169" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L169" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="168" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H168" t="s">
+    <row r="170" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L170" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="169" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H169" t="s">
+    <row r="171" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L171" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="170" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H170" t="s">
+    <row r="172" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L172" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="171" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H171" t="s">
+    <row r="173" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L173" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="172" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H172" t="s">
+    <row r="174" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L174" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="173" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H173" t="s">
+    <row r="175" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L175" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="174" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H174" t="s">
+    <row r="176" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L176" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="175" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H175" t="s">
+    <row r="177" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L177" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="176" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H176" t="s">
+    <row r="178" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L178" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="177" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H177" t="s">
+    <row r="179" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L179" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="178" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H178" t="s">
+    <row r="180" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L180" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="179" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H179" t="s">
+    <row r="181" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L181" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="180" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H180" t="s">
+    <row r="182" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L182" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="181" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H181" t="s">
+    <row r="183" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L183" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="182" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H182" t="s">
+    <row r="184" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L184" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="183" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H183" t="s">
+    <row r="185" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L185" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="184" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H184" t="s">
+    <row r="186" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L186" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="185" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H185" t="s">
+    <row r="187" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L187" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="186" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H186" t="s">
+    <row r="188" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L188" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="187" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H187" t="s">
+    <row r="189" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L189" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="188" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H188" t="s">
+    <row r="190" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L190" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="189" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H189" t="s">
+    <row r="191" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L191" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="190" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H190" t="s">
+    <row r="192" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L192" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="191" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H191" t="s">
+    <row r="193" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L193" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="192" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H192" t="s">
+    <row r="194" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L194" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="193" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H193" t="s">
+    <row r="195" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L195" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="194" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H194" t="s">
+    <row r="196" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L196" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="195" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H195" t="s">
+    <row r="197" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L197" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="196" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H196" t="s">
+    <row r="198" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L198" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="197" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H197" t="s">
+    <row r="199" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L199" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="198" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H198" t="s">
+    <row r="200" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L200" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="199" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H199" t="s">
+    <row r="201" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L201" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="200" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H200" t="s">
+    <row r="202" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L202" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="201" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H201" t="s">
+    <row r="203" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L203" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="202" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H202" t="s">
+    <row r="204" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L204" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="203" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H203" t="s">
+    <row r="205" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L205" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="204" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H204" t="s">
+    <row r="206" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L206" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="205" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H205" t="s">
+    <row r="207" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L207" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="206" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H206" t="s">
+    <row r="208" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L208" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="207" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H207" t="s">
+    <row r="209" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L209" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="208" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H208" t="s">
+    <row r="210" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L210" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="209" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H209" t="s">
+    <row r="211" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L211" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="210" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H210" t="s">
+    <row r="212" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L212" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="211" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H211" t="s">
+    <row r="213" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L213" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="212" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H212" t="s">
+    <row r="214" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L214" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="213" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H213" t="s">
+    <row r="215" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L215" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="214" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H214" t="s">
+    <row r="216" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L216" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="215" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H215" t="s">
+    <row r="217" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L217" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="216" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H216" t="s">
+    <row r="218" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L218" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="217" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H217" t="s">
+    <row r="219" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L219" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="218" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H218" t="s">
+    <row r="220" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L220" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="219" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H219" t="s">
+    <row r="221" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L221" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="220" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H220" t="s">
+    <row r="222" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L222" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="221" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H221" t="s">
+    <row r="223" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L223" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="222" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H222" t="s">
+    <row r="224" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L224" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="223" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H223" t="s">
+    <row r="225" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L225" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="224" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H224" t="s">
+    <row r="226" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L226" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="225" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H225" t="s">
+    <row r="227" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L227" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="226" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H226" t="s">
+    <row r="228" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L228" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="227" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H227" t="s">
+    <row r="229" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L229" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="228" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H228" t="s">
+    <row r="230" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L230" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="229" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H229" t="s">
+    <row r="231" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L231" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="230" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H230" t="s">
+    <row r="232" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L232" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="231" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H231" t="s">
+    <row r="233" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L233" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="232" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H232" t="s">
+    <row r="234" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L234" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="233" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H233" t="s">
+    <row r="235" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L235" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="234" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H234" t="s">
+    <row r="236" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L236" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="235" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H235" t="s">
+    <row r="237" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L237" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="236" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H236" t="s">
+    <row r="238" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L238" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="237" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H237" t="s">
+    <row r="239" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L239" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="238" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H238" t="s">
+    <row r="240" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L240" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="239" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H239" t="s">
+    <row r="241" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L241" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="240" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H240" t="s">
+    <row r="242" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L242" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="241" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H241" t="s">
+    <row r="243" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L243" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="242" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H242" t="s">
+    <row r="244" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L244" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="243" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H243" t="s">
+    <row r="245" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L245" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="244" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H244" t="s">
+    <row r="246" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L246" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="245" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H245" t="s">
+    <row r="247" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L247" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="246" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H246" t="s">
+    <row r="248" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L248" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="247" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H247" t="s">
+    <row r="249" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L249" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="248" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H248" t="s">
+    <row r="250" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L250" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="249" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H249" t="s">
+    <row r="251" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L251" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="250" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H250" t="s">
+    <row r="252" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L252" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="251" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H251" t="s">
+    <row r="253" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L253" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="252" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H252" t="s">
+    <row r="254" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L254" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="253" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H253" t="s">
+    <row r="255" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L255" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="254" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H254" t="s">
+    <row r="256" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L256" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="255" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H255" t="s">
+    <row r="257" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L257" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="256" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H256" t="s">
+    <row r="258" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L258" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="257" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H257" t="s">
+    <row r="259" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L259" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="258" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H258" t="s">
+    <row r="260" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L260" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="259" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H259" t="s">
+    <row r="261" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L261" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="260" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H260" t="s">
+    <row r="262" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L262" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="261" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H261" t="s">
+    <row r="263" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L263" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="262" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H262" t="s">
+    <row r="264" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L264" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="263" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H263" t="s">
+    <row r="265" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L265" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="264" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H264" t="s">
+    <row r="266" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L266" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="265" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H265" t="s">
+    <row r="267" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L267" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="266" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H266" t="s">
+    <row r="268" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L268" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="267" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H267" t="s">
+    <row r="269" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L269" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="268" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H268" t="s">
+    <row r="270" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L270" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="269" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H269" t="s">
+    <row r="271" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L271" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="270" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H270" t="s">
+    <row r="272" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L272" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="271" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H271" t="s">
+    <row r="273" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L273" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="272" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H272" t="s">
+    <row r="274" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L274" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="273" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H273" t="s">
+    <row r="275" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L275" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="274" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H274" t="s">
+    <row r="276" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L276" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="275" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H275" t="s">
+    <row r="277" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L277" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="276" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H276" t="s">
+    <row r="278" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L278" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="277" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H277" t="s">
+    <row r="279" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L279" t="s">
         <v>452</v>
-      </c>
-    </row>
-    <row r="278" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H278" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="279" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H279" t="s">
-        <v>454</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <tableParts count="3">
+  <tableParts count="5">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>